<commit_message>
debut de cas d'usage
</commit_message>
<xml_diff>
--- a/document/projet_td.xlsx
+++ b/document/projet_td.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\Techniques de l'informatique\Tower-Defense-2.0\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1963411\Documents\Tower-Defense-2.0\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7179B295-4FC9-4B37-A0FA-D006B93BB05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304BE5D-E804-4EC4-8882-0B39C1345440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BC00F753-7B3B-42D4-93FD-62A5313F9C45}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BC00F753-7B3B-42D4-93FD-62A5313F9C45}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -2710,6 +2710,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2733,6 +2748,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2750,33 +2777,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3468,22 +3468,22 @@
       </c>
     </row>
     <row r="36" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F36" s="150"/>
-      <c r="G36" s="151"/>
-      <c r="H36" s="151"/>
-      <c r="I36" s="151"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="158"/>
+      <c r="H36" s="158"/>
+      <c r="I36" s="158"/>
     </row>
     <row r="37" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F37" s="151"/>
-      <c r="G37" s="151"/>
-      <c r="H37" s="151"/>
-      <c r="I37" s="151"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="158"/>
+      <c r="H37" s="158"/>
+      <c r="I37" s="158"/>
     </row>
     <row r="38" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F38" s="151"/>
-      <c r="G38" s="151"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="151"/>
+      <c r="F38" s="158"/>
+      <c r="G38" s="158"/>
+      <c r="H38" s="158"/>
+      <c r="I38" s="158"/>
     </row>
     <row r="39" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="102"/>
@@ -3492,22 +3492,22 @@
       <c r="I39" s="102"/>
     </row>
     <row r="40" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F40" s="150"/>
-      <c r="G40" s="151"/>
-      <c r="H40" s="151"/>
-      <c r="I40" s="151"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="158"/>
+      <c r="H40" s="158"/>
+      <c r="I40" s="158"/>
     </row>
     <row r="41" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F41" s="151"/>
-      <c r="G41" s="151"/>
-      <c r="H41" s="151"/>
-      <c r="I41" s="151"/>
+      <c r="F41" s="158"/>
+      <c r="G41" s="158"/>
+      <c r="H41" s="158"/>
+      <c r="I41" s="158"/>
     </row>
     <row r="42" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F42" s="151"/>
-      <c r="G42" s="151"/>
-      <c r="H42" s="151"/>
-      <c r="I42" s="151"/>
+      <c r="F42" s="158"/>
+      <c r="G42" s="158"/>
+      <c r="H42" s="158"/>
+      <c r="I42" s="158"/>
     </row>
     <row r="43" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="102"/>
@@ -3522,34 +3522,34 @@
       <c r="I44" s="102"/>
     </row>
     <row r="45" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F45" s="150"/>
-      <c r="G45" s="151"/>
-      <c r="H45" s="151"/>
-      <c r="I45" s="151"/>
+      <c r="F45" s="157"/>
+      <c r="G45" s="158"/>
+      <c r="H45" s="158"/>
+      <c r="I45" s="158"/>
     </row>
     <row r="46" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F46" s="151"/>
-      <c r="G46" s="151"/>
-      <c r="H46" s="151"/>
-      <c r="I46" s="151"/>
+      <c r="F46" s="158"/>
+      <c r="G46" s="158"/>
+      <c r="H46" s="158"/>
+      <c r="I46" s="158"/>
     </row>
     <row r="47" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F47" s="151"/>
-      <c r="G47" s="151"/>
-      <c r="H47" s="151"/>
-      <c r="I47" s="151"/>
+      <c r="F47" s="158"/>
+      <c r="G47" s="158"/>
+      <c r="H47" s="158"/>
+      <c r="I47" s="158"/>
     </row>
     <row r="48" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F48" s="151"/>
-      <c r="G48" s="151"/>
-      <c r="H48" s="151"/>
-      <c r="I48" s="151"/>
+      <c r="F48" s="158"/>
+      <c r="G48" s="158"/>
+      <c r="H48" s="158"/>
+      <c r="I48" s="158"/>
     </row>
     <row r="49" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F49" s="151"/>
-      <c r="G49" s="151"/>
-      <c r="H49" s="151"/>
-      <c r="I49" s="151"/>
+      <c r="F49" s="158"/>
+      <c r="G49" s="158"/>
+      <c r="H49" s="158"/>
+      <c r="I49" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3669,7 +3669,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="159" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="133" t="s">
@@ -3683,7 +3683,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="153"/>
+      <c r="B14" s="160"/>
       <c r="C14" s="127" t="s">
         <v>240</v>
       </c>
@@ -3695,7 +3695,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="153"/>
+      <c r="B15" s="160"/>
       <c r="C15" s="129" t="s">
         <v>388</v>
       </c>
@@ -3707,7 +3707,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="153"/>
+      <c r="B16" s="160"/>
       <c r="C16" s="127" t="s">
         <v>152</v>
       </c>
@@ -3719,7 +3719,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="153"/>
+      <c r="B17" s="160"/>
       <c r="C17" s="129" t="s">
         <v>390</v>
       </c>
@@ -3731,7 +3731,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="153"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="127" t="s">
         <v>182</v>
       </c>
@@ -3743,7 +3743,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="153"/>
+      <c r="B19" s="160"/>
       <c r="C19" s="127" t="s">
         <v>205</v>
       </c>
@@ -3755,7 +3755,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="153"/>
+      <c r="B20" s="160"/>
       <c r="C20" s="129" t="s">
         <v>425</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="153"/>
+      <c r="B21" s="160"/>
       <c r="C21" s="129" t="s">
         <v>370</v>
       </c>
@@ -3779,7 +3779,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="153"/>
+      <c r="B22" s="160"/>
       <c r="C22" s="129" t="s">
         <v>362</v>
       </c>
@@ -3791,7 +3791,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="153"/>
+      <c r="B23" s="160"/>
       <c r="C23" s="129" t="s">
         <v>352</v>
       </c>
@@ -3803,7 +3803,7 @@
       </c>
     </row>
     <row r="24" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="153"/>
+      <c r="B24" s="160"/>
       <c r="C24" s="127" t="s">
         <v>256</v>
       </c>
@@ -3815,7 +3815,7 @@
       </c>
     </row>
     <row r="25" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="153"/>
+      <c r="B25" s="160"/>
       <c r="C25" s="127" t="s">
         <v>179</v>
       </c>
@@ -3827,7 +3827,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="153"/>
+      <c r="B26" s="160"/>
       <c r="C26" s="129" t="s">
         <v>305</v>
       </c>
@@ -3839,7 +3839,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="153"/>
+      <c r="B27" s="160"/>
       <c r="C27" s="129" t="s">
         <v>373</v>
       </c>
@@ -3851,7 +3851,7 @@
       </c>
     </row>
     <row r="28" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="153"/>
+      <c r="B28" s="160"/>
       <c r="C28" s="127" t="s">
         <v>197</v>
       </c>
@@ -3863,7 +3863,7 @@
       </c>
     </row>
     <row r="29" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="153"/>
+      <c r="B29" s="160"/>
       <c r="C29" s="127" t="s">
         <v>268</v>
       </c>
@@ -3875,7 +3875,7 @@
       </c>
     </row>
     <row r="30" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="153"/>
+      <c r="B30" s="160"/>
       <c r="C30" s="127" t="s">
         <v>235</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
     </row>
     <row r="31" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="153"/>
+      <c r="B31" s="160"/>
       <c r="C31" s="127" t="s">
         <v>159</v>
       </c>
@@ -3899,7 +3899,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="153"/>
+      <c r="B32" s="160"/>
       <c r="C32" s="127" t="s">
         <v>258</v>
       </c>
@@ -3911,7 +3911,7 @@
       </c>
     </row>
     <row r="33" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="153"/>
+      <c r="B33" s="160"/>
       <c r="C33" s="129" t="s">
         <v>258</v>
       </c>
@@ -3923,7 +3923,7 @@
       </c>
     </row>
     <row r="34" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="153"/>
+      <c r="B34" s="160"/>
       <c r="C34" s="127" t="s">
         <v>223</v>
       </c>
@@ -3935,7 +3935,7 @@
       </c>
     </row>
     <row r="35" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="153"/>
+      <c r="B35" s="160"/>
       <c r="C35" s="129" t="s">
         <v>384</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="153"/>
+      <c r="B36" s="160"/>
       <c r="C36" s="127" t="s">
         <v>250</v>
       </c>
@@ -3959,7 +3959,7 @@
       </c>
     </row>
     <row r="37" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="153"/>
+      <c r="B37" s="160"/>
       <c r="C37" s="129" t="s">
         <v>307</v>
       </c>
@@ -3971,7 +3971,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="153"/>
+      <c r="B38" s="160"/>
       <c r="C38" s="129" t="s">
         <v>414</v>
       </c>
@@ -3983,7 +3983,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="153"/>
+      <c r="B39" s="160"/>
       <c r="C39" s="129" t="s">
         <v>369</v>
       </c>
@@ -3995,7 +3995,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="153"/>
+      <c r="B40" s="160"/>
       <c r="C40" s="129" t="s">
         <v>376</v>
       </c>
@@ -4007,7 +4007,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="153"/>
+      <c r="B41" s="160"/>
       <c r="C41" s="129" t="s">
         <v>420</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
     </row>
     <row r="42" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="153"/>
+      <c r="B42" s="160"/>
       <c r="C42" s="129" t="s">
         <v>272</v>
       </c>
@@ -4031,7 +4031,7 @@
       </c>
     </row>
     <row r="43" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="153"/>
+      <c r="B43" s="160"/>
       <c r="C43" s="127" t="s">
         <v>156</v>
       </c>
@@ -4043,7 +4043,7 @@
       </c>
     </row>
     <row r="44" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="153"/>
+      <c r="B44" s="160"/>
       <c r="C44" s="127" t="s">
         <v>270</v>
       </c>
@@ -4055,7 +4055,7 @@
       </c>
     </row>
     <row r="45" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="153"/>
+      <c r="B45" s="160"/>
       <c r="C45" s="129" t="s">
         <v>304</v>
       </c>
@@ -4067,7 +4067,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="153"/>
+      <c r="B46" s="160"/>
       <c r="C46" s="127" t="s">
         <v>252</v>
       </c>
@@ -4079,7 +4079,7 @@
       </c>
     </row>
     <row r="47" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="153"/>
+      <c r="B47" s="160"/>
       <c r="C47" s="129" t="s">
         <v>311</v>
       </c>
@@ -4091,7 +4091,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="153"/>
+      <c r="B48" s="160"/>
       <c r="C48" s="129" t="s">
         <v>429</v>
       </c>
@@ -4103,7 +4103,7 @@
       </c>
     </row>
     <row r="49" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="153"/>
+      <c r="B49" s="160"/>
       <c r="C49" s="129" t="s">
         <v>350</v>
       </c>
@@ -4115,7 +4115,7 @@
       </c>
     </row>
     <row r="50" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="153"/>
+      <c r="B50" s="160"/>
       <c r="C50" s="127" t="s">
         <v>220</v>
       </c>
@@ -4127,7 +4127,7 @@
       </c>
     </row>
     <row r="51" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="153"/>
+      <c r="B51" s="160"/>
       <c r="C51" s="129" t="s">
         <v>383</v>
       </c>
@@ -4139,7 +4139,7 @@
       </c>
     </row>
     <row r="52" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="153"/>
+      <c r="B52" s="160"/>
       <c r="C52" s="129" t="s">
         <v>378</v>
       </c>
@@ -4151,7 +4151,7 @@
       </c>
     </row>
     <row r="53" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="153"/>
+      <c r="B53" s="160"/>
       <c r="C53" s="127" t="s">
         <v>188</v>
       </c>
@@ -4163,7 +4163,7 @@
       </c>
     </row>
     <row r="54" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="153"/>
+      <c r="B54" s="160"/>
       <c r="C54" s="129" t="s">
         <v>293</v>
       </c>
@@ -4175,7 +4175,7 @@
       </c>
     </row>
     <row r="55" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="153"/>
+      <c r="B55" s="160"/>
       <c r="C55" s="129" t="s">
         <v>351</v>
       </c>
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="56" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="153"/>
+      <c r="B56" s="160"/>
       <c r="C56" s="129" t="s">
         <v>377</v>
       </c>
@@ -4199,7 +4199,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="153"/>
+      <c r="B57" s="160"/>
       <c r="C57" s="129" t="s">
         <v>400</v>
       </c>
@@ -4211,7 +4211,7 @@
       </c>
     </row>
     <row r="58" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="153"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="129" t="s">
         <v>292</v>
       </c>
@@ -4223,7 +4223,7 @@
       </c>
     </row>
     <row r="59" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="153"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="129" t="s">
         <v>375</v>
       </c>
@@ -4235,7 +4235,7 @@
       </c>
     </row>
     <row r="60" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="153"/>
+      <c r="B60" s="160"/>
       <c r="C60" s="127" t="s">
         <v>176</v>
       </c>
@@ -4247,7 +4247,7 @@
       </c>
     </row>
     <row r="61" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="153"/>
+      <c r="B61" s="160"/>
       <c r="C61" s="127" t="s">
         <v>262</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
     </row>
     <row r="62" spans="2:5" s="123" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="153"/>
+      <c r="B62" s="160"/>
       <c r="C62" s="129" t="s">
         <v>196</v>
       </c>
@@ -4271,7 +4271,7 @@
       </c>
     </row>
     <row r="63" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="153"/>
+      <c r="B63" s="160"/>
       <c r="C63" s="129" t="s">
         <v>285</v>
       </c>
@@ -4283,7 +4283,7 @@
       </c>
     </row>
     <row r="64" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="153"/>
+      <c r="B64" s="160"/>
       <c r="C64" s="129" t="s">
         <v>353</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
     </row>
     <row r="65" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="153"/>
+      <c r="B65" s="160"/>
       <c r="C65" s="129" t="s">
         <v>297</v>
       </c>
@@ -4307,7 +4307,7 @@
       </c>
     </row>
     <row r="66" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="153"/>
+      <c r="B66" s="160"/>
       <c r="C66" s="129" t="s">
         <v>295</v>
       </c>
@@ -4319,7 +4319,7 @@
       </c>
     </row>
     <row r="67" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="153"/>
+      <c r="B67" s="160"/>
       <c r="C67" s="129" t="s">
         <v>289</v>
       </c>
@@ -4331,7 +4331,7 @@
       </c>
     </row>
     <row r="68" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="153"/>
+      <c r="B68" s="160"/>
       <c r="C68" s="127" t="s">
         <v>261</v>
       </c>
@@ -4343,7 +4343,7 @@
       </c>
     </row>
     <row r="69" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="153"/>
+      <c r="B69" s="160"/>
       <c r="C69" s="129" t="s">
         <v>426</v>
       </c>
@@ -4355,7 +4355,7 @@
       </c>
     </row>
     <row r="70" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="153"/>
+      <c r="B70" s="160"/>
       <c r="C70" s="127" t="s">
         <v>194</v>
       </c>
@@ -4367,7 +4367,7 @@
       </c>
     </row>
     <row r="71" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="153"/>
+      <c r="B71" s="160"/>
       <c r="C71" s="127" t="s">
         <v>165</v>
       </c>
@@ -4379,7 +4379,7 @@
       </c>
     </row>
     <row r="72" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="153"/>
+      <c r="B72" s="160"/>
       <c r="C72" s="127" t="s">
         <v>255</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
     </row>
     <row r="73" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="153"/>
+      <c r="B73" s="160"/>
       <c r="C73" s="129" t="s">
         <v>315</v>
       </c>
@@ -4403,7 +4403,7 @@
       </c>
     </row>
     <row r="74" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="153"/>
+      <c r="B74" s="160"/>
       <c r="C74" s="127" t="s">
         <v>260</v>
       </c>
@@ -4415,7 +4415,7 @@
       </c>
     </row>
     <row r="75" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="153"/>
+      <c r="B75" s="160"/>
       <c r="C75" s="127" t="s">
         <v>214</v>
       </c>
@@ -4427,7 +4427,7 @@
       </c>
     </row>
     <row r="76" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="153"/>
+      <c r="B76" s="160"/>
       <c r="C76" s="127" t="s">
         <v>226</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
     </row>
     <row r="77" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="153"/>
+      <c r="B77" s="160"/>
       <c r="C77" s="129" t="s">
         <v>347</v>
       </c>
@@ -4451,7 +4451,7 @@
       </c>
     </row>
     <row r="78" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="153"/>
+      <c r="B78" s="160"/>
       <c r="C78" s="127" t="s">
         <v>265</v>
       </c>
@@ -4463,7 +4463,7 @@
       </c>
     </row>
     <row r="79" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="153"/>
+      <c r="B79" s="160"/>
       <c r="C79" s="129" t="s">
         <v>325</v>
       </c>
@@ -4475,7 +4475,7 @@
       </c>
     </row>
     <row r="80" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="153"/>
+      <c r="B80" s="160"/>
       <c r="C80" s="129" t="s">
         <v>296</v>
       </c>
@@ -4487,7 +4487,7 @@
       </c>
     </row>
     <row r="81" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="153"/>
+      <c r="B81" s="160"/>
       <c r="C81" s="129" t="s">
         <v>74</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
     </row>
     <row r="82" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="154"/>
+      <c r="B82" s="161"/>
       <c r="C82" s="127" t="s">
         <v>269</v>
       </c>
@@ -4511,7 +4511,7 @@
       </c>
     </row>
     <row r="83" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="154"/>
+      <c r="B83" s="161"/>
       <c r="C83" s="129" t="s">
         <v>394</v>
       </c>
@@ -4523,7 +4523,7 @@
       </c>
     </row>
     <row r="84" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="154"/>
+      <c r="B84" s="161"/>
       <c r="C84" s="129" t="s">
         <v>380</v>
       </c>
@@ -4535,7 +4535,7 @@
       </c>
     </row>
     <row r="85" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="154"/>
+      <c r="B85" s="161"/>
       <c r="C85" s="127" t="s">
         <v>208</v>
       </c>
@@ -4547,7 +4547,7 @@
       </c>
     </row>
     <row r="86" spans="2:5" s="122" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="154"/>
+      <c r="B86" s="161"/>
       <c r="C86" s="127" t="s">
         <v>276</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="154"/>
+      <c r="B87" s="161"/>
       <c r="C87" s="127" t="s">
         <v>173</v>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
     </row>
     <row r="88" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="154"/>
+      <c r="B88" s="161"/>
       <c r="C88" s="127" t="s">
         <v>248</v>
       </c>
@@ -4583,7 +4583,7 @@
       </c>
     </row>
     <row r="89" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="154"/>
+      <c r="B89" s="161"/>
       <c r="C89" s="129" t="s">
         <v>323</v>
       </c>
@@ -4595,7 +4595,7 @@
       </c>
     </row>
     <row r="90" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="154"/>
+      <c r="B90" s="161"/>
       <c r="C90" s="127" t="s">
         <v>232</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="E90" s="131"/>
     </row>
     <row r="91" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="154"/>
+      <c r="B91" s="161"/>
       <c r="C91" s="129" t="s">
         <v>232</v>
       </c>
@@ -4615,7 +4615,7 @@
       <c r="E91" s="131"/>
     </row>
     <row r="92" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="154"/>
+      <c r="B92" s="161"/>
       <c r="C92" s="127" t="s">
         <v>246</v>
       </c>
@@ -4625,7 +4625,7 @@
       <c r="E92" s="131"/>
     </row>
     <row r="93" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="154"/>
+      <c r="B93" s="161"/>
       <c r="C93" s="129" t="s">
         <v>374</v>
       </c>
@@ -4635,7 +4635,7 @@
       <c r="E93" s="131"/>
     </row>
     <row r="94" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="154"/>
+      <c r="B94" s="161"/>
       <c r="C94" s="127" t="s">
         <v>264</v>
       </c>
@@ -4645,7 +4645,7 @@
       <c r="E94" s="131"/>
     </row>
     <row r="95" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="154"/>
+      <c r="B95" s="161"/>
       <c r="C95" s="128" t="s">
         <v>412</v>
       </c>
@@ -4653,7 +4653,7 @@
       <c r="E95" s="125"/>
     </row>
     <row r="96" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="154"/>
+      <c r="B96" s="161"/>
       <c r="C96" s="129" t="s">
         <v>282</v>
       </c>
@@ -4661,7 +4661,7 @@
       <c r="E96" s="131"/>
     </row>
     <row r="97" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="154"/>
+      <c r="B97" s="161"/>
       <c r="C97" s="129" t="s">
         <v>334</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="E97" s="131"/>
     </row>
     <row r="98" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="154"/>
+      <c r="B98" s="161"/>
       <c r="C98" s="129" t="s">
         <v>340</v>
       </c>
@@ -4677,7 +4677,7 @@
       <c r="E98" s="131"/>
     </row>
     <row r="99" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="154"/>
+      <c r="B99" s="161"/>
       <c r="C99" s="129" t="s">
         <v>359</v>
       </c>
@@ -4685,7 +4685,7 @@
       <c r="E99" s="131"/>
     </row>
     <row r="100" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="154"/>
+      <c r="B100" s="161"/>
       <c r="C100" s="129" t="s">
         <v>367</v>
       </c>
@@ -4693,7 +4693,7 @@
       <c r="E100" s="131"/>
     </row>
     <row r="101" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="154"/>
+      <c r="B101" s="161"/>
       <c r="C101" s="129" t="s">
         <v>318</v>
       </c>
@@ -4701,7 +4701,7 @@
       <c r="E101" s="131"/>
     </row>
     <row r="102" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="154"/>
+      <c r="B102" s="161"/>
       <c r="C102" s="127" t="s">
         <v>211</v>
       </c>
@@ -4709,7 +4709,7 @@
       <c r="E102" s="131"/>
     </row>
     <row r="103" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="154"/>
+      <c r="B103" s="161"/>
       <c r="C103" s="129" t="s">
         <v>354</v>
       </c>
@@ -4717,7 +4717,7 @@
       <c r="E103" s="131"/>
     </row>
     <row r="104" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="154"/>
+      <c r="B104" s="161"/>
       <c r="C104" s="127" t="s">
         <v>200</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="E104" s="131"/>
     </row>
     <row r="105" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="154"/>
+      <c r="B105" s="161"/>
       <c r="C105" s="127" t="s">
         <v>243</v>
       </c>
@@ -4733,7 +4733,7 @@
       <c r="E105" s="131"/>
     </row>
     <row r="106" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="154"/>
+      <c r="B106" s="161"/>
       <c r="C106" s="129" t="s">
         <v>387</v>
       </c>
@@ -4741,7 +4741,7 @@
       <c r="E106" s="131"/>
     </row>
     <row r="107" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="154"/>
+      <c r="B107" s="161"/>
       <c r="C107" s="127" t="s">
         <v>257</v>
       </c>
@@ -4749,7 +4749,7 @@
       <c r="E107" s="131"/>
     </row>
     <row r="108" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="154"/>
+      <c r="B108" s="161"/>
       <c r="C108" s="127" t="s">
         <v>254</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="E108" s="131"/>
     </row>
     <row r="109" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="154"/>
+      <c r="B109" s="161"/>
       <c r="C109" s="127" t="s">
         <v>266</v>
       </c>
@@ -4765,7 +4765,7 @@
       <c r="E109" s="131"/>
     </row>
     <row r="110" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="154"/>
+      <c r="B110" s="161"/>
       <c r="C110" s="129" t="s">
         <v>345</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="E110" s="131"/>
     </row>
     <row r="111" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="154"/>
+      <c r="B111" s="161"/>
       <c r="C111" s="129" t="s">
         <v>151</v>
       </c>
@@ -4781,7 +4781,7 @@
       <c r="E111" s="131"/>
     </row>
     <row r="112" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="154"/>
+      <c r="B112" s="161"/>
       <c r="C112" s="127" t="s">
         <v>267</v>
       </c>
@@ -4789,7 +4789,7 @@
       <c r="E112" s="131"/>
     </row>
     <row r="113" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="154"/>
+      <c r="B113" s="161"/>
       <c r="C113" s="129" t="s">
         <v>357</v>
       </c>
@@ -4797,7 +4797,7 @@
       <c r="E113" s="131"/>
     </row>
     <row r="114" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B114" s="154"/>
+      <c r="B114" s="161"/>
       <c r="C114" s="129" t="s">
         <v>339</v>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="E114" s="131"/>
     </row>
     <row r="115" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="154"/>
+      <c r="B115" s="161"/>
       <c r="C115" s="127" t="s">
         <v>263</v>
       </c>
@@ -4813,7 +4813,7 @@
       <c r="E115" s="131"/>
     </row>
     <row r="116" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B116" s="154"/>
+      <c r="B116" s="161"/>
       <c r="C116" s="127" t="s">
         <v>162</v>
       </c>
@@ -4821,7 +4821,7 @@
       <c r="E116" s="131"/>
     </row>
     <row r="117" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B117" s="154"/>
+      <c r="B117" s="161"/>
       <c r="C117" s="129" t="s">
         <v>349</v>
       </c>
@@ -4829,7 +4829,7 @@
       <c r="E117" s="131"/>
     </row>
     <row r="118" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="154"/>
+      <c r="B118" s="161"/>
       <c r="C118" s="129" t="s">
         <v>324</v>
       </c>
@@ -4837,7 +4837,7 @@
       <c r="E118" s="131"/>
     </row>
     <row r="119" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B119" s="154"/>
+      <c r="B119" s="161"/>
       <c r="C119" s="129" t="s">
         <v>332</v>
       </c>
@@ -4845,7 +4845,7 @@
       <c r="E119" s="131"/>
     </row>
     <row r="120" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B120" s="154"/>
+      <c r="B120" s="161"/>
       <c r="C120" s="127" t="s">
         <v>185</v>
       </c>
@@ -4853,7 +4853,7 @@
       <c r="E120" s="131"/>
     </row>
     <row r="121" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="154"/>
+      <c r="B121" s="161"/>
       <c r="C121" s="129" t="s">
         <v>309</v>
       </c>
@@ -4861,7 +4861,7 @@
       <c r="E121" s="131"/>
     </row>
     <row r="122" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="154"/>
+      <c r="B122" s="161"/>
       <c r="C122" s="127" t="s">
         <v>191</v>
       </c>
@@ -4869,7 +4869,7 @@
       <c r="E122" s="131"/>
     </row>
     <row r="123" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="154"/>
+      <c r="B123" s="161"/>
       <c r="C123" s="129" t="s">
         <v>191</v>
       </c>
@@ -4877,7 +4877,7 @@
       <c r="E123" s="131"/>
     </row>
     <row r="124" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="154"/>
+      <c r="B124" s="161"/>
       <c r="C124" s="129" t="s">
         <v>294</v>
       </c>
@@ -4885,7 +4885,7 @@
       <c r="E124" s="131"/>
     </row>
     <row r="125" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="154"/>
+      <c r="B125" s="161"/>
       <c r="C125" s="127" t="s">
         <v>229</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="E125" s="131"/>
     </row>
     <row r="126" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B126" s="154"/>
+      <c r="B126" s="161"/>
       <c r="C126" s="127" t="s">
         <v>217</v>
       </c>
@@ -4901,7 +4901,7 @@
       <c r="E126" s="131"/>
     </row>
     <row r="127" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="154"/>
+      <c r="B127" s="161"/>
       <c r="C127" s="127" t="s">
         <v>237</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="E127" s="131"/>
     </row>
     <row r="128" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="154"/>
+      <c r="B128" s="161"/>
       <c r="C128" s="127" t="s">
         <v>168</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="E128" s="131"/>
     </row>
     <row r="129" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B129" s="154"/>
+      <c r="B129" s="161"/>
       <c r="C129" s="127" t="s">
         <v>271</v>
       </c>
@@ -4925,7 +4925,7 @@
       <c r="E129" s="131"/>
     </row>
     <row r="130" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B130" s="154"/>
+      <c r="B130" s="161"/>
       <c r="C130" s="129" t="s">
         <v>381</v>
       </c>
@@ -4933,7 +4933,7 @@
       <c r="E130" s="131"/>
     </row>
     <row r="131" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B131" s="154"/>
+      <c r="B131" s="161"/>
       <c r="C131" s="129" t="s">
         <v>286</v>
       </c>
@@ -4941,7 +4941,7 @@
       <c r="E131" s="131"/>
     </row>
     <row r="132" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="154"/>
+      <c r="B132" s="161"/>
       <c r="C132" s="129" t="s">
         <v>392</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="E132" s="131"/>
     </row>
     <row r="133" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="154"/>
+      <c r="B133" s="161"/>
       <c r="C133" s="129" t="s">
         <v>327</v>
       </c>
@@ -4957,7 +4957,7 @@
       <c r="E133" s="131"/>
     </row>
     <row r="134" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="154"/>
+      <c r="B134" s="161"/>
       <c r="C134" s="129" t="s">
         <v>283</v>
       </c>
@@ -4965,7 +4965,7 @@
       <c r="E134" s="131"/>
     </row>
     <row r="135" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B135" s="154"/>
+      <c r="B135" s="161"/>
       <c r="C135" s="127" t="s">
         <v>259</v>
       </c>
@@ -4973,7 +4973,7 @@
       <c r="E135" s="131"/>
     </row>
     <row r="136" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="154"/>
+      <c r="B136" s="161"/>
       <c r="C136" s="129" t="s">
         <v>199</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="E136" s="131"/>
     </row>
     <row r="137" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="154"/>
+      <c r="B137" s="161"/>
       <c r="C137" s="129" t="s">
         <v>372</v>
       </c>
@@ -4989,7 +4989,7 @@
       <c r="E137" s="131"/>
     </row>
     <row r="138" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B138" s="154"/>
+      <c r="B138" s="161"/>
       <c r="C138" s="129" t="s">
         <v>398</v>
       </c>
@@ -4997,79 +4997,79 @@
       <c r="E138" s="131"/>
     </row>
     <row r="139" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B139" s="154"/>
+      <c r="B139" s="161"/>
       <c r="C139" s="129"/>
       <c r="D139" s="125"/>
       <c r="E139" s="131"/>
     </row>
     <row r="140" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B140" s="154"/>
+      <c r="B140" s="161"/>
       <c r="C140" s="129"/>
       <c r="D140" s="125"/>
       <c r="E140" s="131"/>
     </row>
     <row r="141" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B141" s="154"/>
+      <c r="B141" s="161"/>
       <c r="C141" s="129"/>
       <c r="D141" s="125"/>
       <c r="E141" s="131"/>
     </row>
     <row r="142" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="154"/>
+      <c r="B142" s="161"/>
       <c r="C142" s="129"/>
       <c r="D142" s="125"/>
       <c r="E142" s="131"/>
     </row>
     <row r="143" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B143" s="154"/>
+      <c r="B143" s="161"/>
       <c r="C143" s="129"/>
       <c r="D143" s="125"/>
       <c r="E143" s="131"/>
     </row>
     <row r="144" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B144" s="154"/>
+      <c r="B144" s="161"/>
       <c r="C144" s="129"/>
       <c r="D144" s="125"/>
       <c r="E144" s="131"/>
     </row>
     <row r="145" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B145" s="154"/>
+      <c r="B145" s="161"/>
       <c r="C145" s="129"/>
       <c r="D145" s="125"/>
       <c r="E145" s="131"/>
     </row>
     <row r="146" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B146" s="154"/>
+      <c r="B146" s="161"/>
       <c r="C146" s="129"/>
       <c r="D146" s="125"/>
       <c r="E146" s="131"/>
     </row>
     <row r="147" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B147" s="154"/>
+      <c r="B147" s="161"/>
       <c r="C147" s="129"/>
       <c r="D147" s="125"/>
       <c r="E147" s="131"/>
     </row>
     <row r="148" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="154"/>
+      <c r="B148" s="161"/>
       <c r="C148" s="129"/>
       <c r="D148" s="125"/>
       <c r="E148" s="131"/>
     </row>
     <row r="149" spans="2:5" s="124" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B149" s="154"/>
+      <c r="B149" s="161"/>
       <c r="C149" s="129"/>
       <c r="D149" s="125"/>
       <c r="E149" s="131"/>
     </row>
     <row r="150" spans="2:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="154"/>
+      <c r="B150" s="161"/>
       <c r="C150" s="129"/>
       <c r="D150" s="125"/>
       <c r="E150" s="131"/>
     </row>
     <row r="151" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="152" t="s">
+      <c r="B151" s="159" t="s">
         <v>60</v>
       </c>
       <c r="C151" s="133" t="s">
@@ -5079,7 +5079,7 @@
       <c r="E151" s="134"/>
     </row>
     <row r="152" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B152" s="154"/>
+      <c r="B152" s="161"/>
       <c r="C152" s="129" t="s">
         <v>401</v>
       </c>
@@ -5087,49 +5087,49 @@
       <c r="E152" s="131"/>
     </row>
     <row r="153" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B153" s="154"/>
+      <c r="B153" s="161"/>
       <c r="C153" s="129"/>
       <c r="D153" s="125"/>
       <c r="E153" s="131"/>
     </row>
     <row r="154" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="154"/>
+      <c r="B154" s="161"/>
       <c r="C154" s="129"/>
       <c r="D154" s="125"/>
       <c r="E154" s="131"/>
     </row>
     <row r="155" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B155" s="154"/>
+      <c r="B155" s="161"/>
       <c r="C155" s="129"/>
       <c r="D155" s="125"/>
       <c r="E155" s="131"/>
     </row>
     <row r="156" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B156" s="154"/>
+      <c r="B156" s="161"/>
       <c r="C156" s="129"/>
       <c r="D156" s="125"/>
       <c r="E156" s="131"/>
     </row>
     <row r="157" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B157" s="154"/>
+      <c r="B157" s="161"/>
       <c r="C157" s="129"/>
       <c r="D157" s="125"/>
       <c r="E157" s="131"/>
     </row>
     <row r="158" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B158" s="154"/>
+      <c r="B158" s="161"/>
       <c r="C158" s="129"/>
       <c r="D158" s="125"/>
       <c r="E158" s="131"/>
     </row>
     <row r="159" spans="2:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="155"/>
+      <c r="B159" s="162"/>
       <c r="C159" s="135"/>
       <c r="D159" s="140"/>
       <c r="E159" s="132"/>
     </row>
     <row r="160" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B160" s="152" t="s">
+      <c r="B160" s="159" t="s">
         <v>61</v>
       </c>
       <c r="C160" s="133"/>
@@ -5137,55 +5137,55 @@
       <c r="E160" s="134"/>
     </row>
     <row r="161" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B161" s="154"/>
+      <c r="B161" s="161"/>
       <c r="C161" s="129"/>
       <c r="D161" s="125"/>
       <c r="E161" s="131"/>
     </row>
     <row r="162" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B162" s="154"/>
+      <c r="B162" s="161"/>
       <c r="C162" s="129"/>
       <c r="D162" s="125"/>
       <c r="E162" s="131"/>
     </row>
     <row r="163" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B163" s="154"/>
+      <c r="B163" s="161"/>
       <c r="C163" s="129"/>
       <c r="D163" s="125"/>
       <c r="E163" s="131"/>
     </row>
     <row r="164" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="154"/>
+      <c r="B164" s="161"/>
       <c r="C164" s="129"/>
       <c r="D164" s="125"/>
       <c r="E164" s="131"/>
     </row>
     <row r="165" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B165" s="154"/>
+      <c r="B165" s="161"/>
       <c r="C165" s="129"/>
       <c r="D165" s="125"/>
       <c r="E165" s="131"/>
     </row>
     <row r="166" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="154"/>
+      <c r="B166" s="161"/>
       <c r="C166" s="129"/>
       <c r="D166" s="125"/>
       <c r="E166" s="131"/>
     </row>
     <row r="167" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B167" s="154"/>
+      <c r="B167" s="161"/>
       <c r="C167" s="129"/>
       <c r="D167" s="125"/>
       <c r="E167" s="131"/>
     </row>
     <row r="168" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B168" s="154"/>
+      <c r="B168" s="161"/>
       <c r="C168" s="127"/>
       <c r="D168" s="125"/>
       <c r="E168" s="131"/>
     </row>
     <row r="169" spans="2:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="155"/>
+      <c r="B169" s="162"/>
       <c r="C169" s="136"/>
       <c r="D169" s="140"/>
       <c r="E169" s="132"/>
@@ -5211,8 +5211,8 @@
   </sheetPr>
   <dimension ref="B2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5239,22 +5239,22 @@
     </row>
     <row r="3" spans="2:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="99"/>
-      <c r="C3" s="156" t="s">
+      <c r="C3" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="156"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
       <c r="G3" s="99"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="100"/>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="157"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
       <c r="G4" s="100"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5321,7 +5321,7 @@
       <c r="B11" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="166" t="s">
+      <c r="C11" s="152" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="149" t="s">
@@ -5338,7 +5338,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="164"/>
+      <c r="B12" s="150"/>
       <c r="C12" s="167" t="s">
         <v>432</v>
       </c>
@@ -5352,72 +5352,72 @@
       </c>
     </row>
     <row r="13" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="164"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="172"/>
+      <c r="B13" s="150"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="154"/>
       <c r="E13" s="29"/>
       <c r="F13" s="45"/>
       <c r="G13" s="145"/>
     </row>
     <row r="14" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="164"/>
-      <c r="C14" s="171"/>
-      <c r="D14" s="172"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="153"/>
+      <c r="D14" s="154"/>
       <c r="E14" s="29"/>
       <c r="F14" s="45"/>
       <c r="G14" s="145"/>
     </row>
     <row r="15" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="164"/>
-      <c r="C15" s="171"/>
-      <c r="D15" s="172"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="153"/>
+      <c r="D15" s="154"/>
       <c r="E15" s="29"/>
       <c r="F15" s="45"/>
       <c r="G15" s="145"/>
     </row>
     <row r="16" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="164"/>
-      <c r="C16" s="171"/>
-      <c r="D16" s="172"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="153"/>
+      <c r="D16" s="154"/>
       <c r="E16" s="29"/>
       <c r="F16" s="45"/>
       <c r="G16" s="145"/>
     </row>
     <row r="17" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="164"/>
-      <c r="C17" s="171"/>
-      <c r="D17" s="172"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="153"/>
+      <c r="D17" s="154"/>
       <c r="E17" s="29"/>
       <c r="F17" s="45"/>
       <c r="G17" s="145"/>
     </row>
     <row r="18" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="164"/>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="153"/>
+      <c r="D18" s="154"/>
       <c r="E18" s="29"/>
       <c r="F18" s="45"/>
       <c r="G18" s="145"/>
     </row>
     <row r="19" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="164"/>
-      <c r="C19" s="171"/>
-      <c r="D19" s="172"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="153"/>
+      <c r="D19" s="154"/>
       <c r="E19" s="29"/>
       <c r="F19" s="45"/>
       <c r="G19" s="145"/>
     </row>
     <row r="20" spans="2:7" s="144" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="164"/>
-      <c r="C20" s="171"/>
-      <c r="D20" s="172"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="153"/>
+      <c r="D20" s="154"/>
       <c r="E20" s="29"/>
       <c r="F20" s="45"/>
       <c r="G20" s="145"/>
     </row>
     <row r="21" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="164"/>
-      <c r="C21" s="173"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="155"/>
       <c r="D21" s="148"/>
       <c r="E21" s="148"/>
       <c r="F21" s="21"/>
@@ -5426,64 +5426,64 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="165"/>
-      <c r="C22" s="169" t="s">
+      <c r="B22" s="151"/>
+      <c r="C22" s="165" t="s">
         <v>441</v>
       </c>
-      <c r="D22" s="170"/>
+      <c r="D22" s="166"/>
       <c r="E22" s="148"/>
       <c r="F22" s="148"/>
     </row>
     <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="165"/>
-      <c r="C23" s="173"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="155"/>
       <c r="D23" s="148"/>
       <c r="E23" s="148"/>
       <c r="F23" s="148"/>
     </row>
     <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="165"/>
-      <c r="C24" s="169" t="s">
+      <c r="B24" s="151"/>
+      <c r="C24" s="165" t="s">
         <v>440</v>
       </c>
-      <c r="D24" s="170"/>
+      <c r="D24" s="166"/>
       <c r="E24" s="148"/>
       <c r="F24" s="148"/>
     </row>
     <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="165"/>
-      <c r="C25" s="173"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="155"/>
       <c r="D25" s="148"/>
       <c r="E25" s="148"/>
       <c r="F25" s="148"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="165"/>
-      <c r="C26" s="169" t="s">
+      <c r="B26" s="151"/>
+      <c r="C26" s="165" t="s">
         <v>442</v>
       </c>
-      <c r="D26" s="170"/>
+      <c r="D26" s="166"/>
       <c r="E26" s="148"/>
       <c r="F26" s="148"/>
     </row>
     <row r="27" spans="2:7" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="165"/>
-      <c r="C27" s="174"/>
+      <c r="B27" s="151"/>
+      <c r="C27" s="156"/>
       <c r="D27" s="148"/>
       <c r="E27" s="148"/>
       <c r="F27" s="148"/>
     </row>
     <row r="28" spans="2:7" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="165"/>
-      <c r="C28" s="169" t="s">
+      <c r="B28" s="151"/>
+      <c r="C28" s="165" t="s">
         <v>444</v>
       </c>
-      <c r="D28" s="170"/>
+      <c r="D28" s="166"/>
       <c r="E28" s="148"/>
       <c r="F28" s="148"/>
     </row>
     <row r="29" spans="2:7" s="144" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="165"/>
+      <c r="B29" s="151"/>
       <c r="C29" s="148"/>
       <c r="D29" s="148" t="s">
         <v>434</v>
@@ -5492,7 +5492,7 @@
       <c r="F29" s="148"/>
     </row>
     <row r="30" spans="2:7" s="144" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="165"/>
+      <c r="B30" s="151"/>
       <c r="C30" s="148"/>
       <c r="D30" s="148" t="s">
         <v>435</v>
@@ -5501,7 +5501,7 @@
       <c r="F30" s="148"/>
     </row>
     <row r="31" spans="2:7" s="144" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B31" s="165"/>
+      <c r="B31" s="151"/>
       <c r="C31" s="148"/>
       <c r="D31" s="148" t="s">
         <v>436</v>
@@ -5510,7 +5510,7 @@
       <c r="F31" s="148"/>
     </row>
     <row r="32" spans="2:7" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="165"/>
+      <c r="B32" s="151"/>
       <c r="C32" s="148"/>
       <c r="D32" s="148" t="s">
         <v>437</v>
@@ -5519,7 +5519,7 @@
       <c r="F32" s="148"/>
     </row>
     <row r="33" spans="2:6" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="165"/>
+      <c r="B33" s="151"/>
       <c r="C33" s="148"/>
       <c r="D33" s="148" t="s">
         <v>438</v>
@@ -5528,7 +5528,7 @@
       <c r="F33" s="148"/>
     </row>
     <row r="34" spans="2:6" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="165"/>
+      <c r="B34" s="151"/>
       <c r="C34" s="148"/>
       <c r="D34" s="148" t="s">
         <v>445</v>
@@ -5537,7 +5537,7 @@
       <c r="F34" s="148"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="165"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="148"/>
       <c r="D35" s="148" t="s">
         <v>439</v>
@@ -5546,39 +5546,39 @@
       <c r="F35" s="148"/>
     </row>
     <row r="36" spans="2:6" s="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="165"/>
-      <c r="C36" s="174"/>
+      <c r="B36" s="151"/>
+      <c r="C36" s="156"/>
       <c r="D36" s="148"/>
       <c r="E36" s="148"/>
       <c r="F36" s="148"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="165"/>
-      <c r="C37" s="169" t="s">
+      <c r="B37" s="151"/>
+      <c r="C37" s="165" t="s">
         <v>446</v>
       </c>
-      <c r="D37" s="170"/>
+      <c r="D37" s="166"/>
       <c r="E37" s="148"/>
       <c r="F37" s="148"/>
     </row>
     <row r="38" spans="2:6" s="126" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="165"/>
-      <c r="C38" s="174"/>
+      <c r="B38" s="151"/>
+      <c r="C38" s="156"/>
       <c r="D38" s="148"/>
       <c r="E38" s="148"/>
       <c r="F38" s="148"/>
     </row>
     <row r="39" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B39" s="165"/>
-      <c r="C39" s="169" t="s">
+      <c r="B39" s="151"/>
+      <c r="C39" s="165" t="s">
         <v>443</v>
       </c>
-      <c r="D39" s="170"/>
+      <c r="D39" s="166"/>
       <c r="E39" s="148"/>
       <c r="F39" s="148"/>
     </row>
     <row r="40" spans="2:6" s="126" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="165"/>
+      <c r="B40" s="151"/>
       <c r="C40" s="148"/>
       <c r="D40" s="148" t="s">
         <v>447</v>
@@ -5587,7 +5587,7 @@
       <c r="F40" s="148"/>
     </row>
     <row r="41" spans="2:6" s="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="165"/>
+      <c r="B41" s="151"/>
       <c r="C41" s="148"/>
       <c r="D41" s="148" t="s">
         <v>448</v>
@@ -5596,7 +5596,7 @@
       <c r="F41" s="148"/>
     </row>
     <row r="42" spans="2:6" s="126" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="165"/>
+      <c r="B42" s="151"/>
       <c r="C42" s="148"/>
       <c r="D42" s="148" t="s">
         <v>449</v>
@@ -5605,7 +5605,7 @@
       <c r="F42" s="148"/>
     </row>
     <row r="43" spans="2:6" s="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="165"/>
+      <c r="B43" s="151"/>
       <c r="C43" s="148"/>
       <c r="D43" s="148" t="s">
         <v>450</v>
@@ -5831,13 +5831,13 @@
       <c r="J11" s="102"/>
       <c r="K11" s="102"/>
       <c r="L11" s="102"/>
-      <c r="M11" s="159"/>
-      <c r="N11" s="151"/>
-      <c r="O11" s="151"/>
+      <c r="M11" s="170"/>
+      <c r="N11" s="158"/>
+      <c r="O11" s="158"/>
       <c r="P11" s="102"/>
       <c r="Q11" s="102"/>
-      <c r="R11" s="159"/>
-      <c r="S11" s="160"/>
+      <c r="R11" s="170"/>
+      <c r="S11" s="171"/>
     </row>
     <row r="12" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G12" s="27"/>
@@ -6043,9 +6043,9 @@
       <c r="W23" s="102"/>
     </row>
     <row r="24" spans="7:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="G24" s="158"/>
-      <c r="H24" s="151"/>
-      <c r="I24" s="151"/>
+      <c r="G24" s="169"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="158"/>
       <c r="J24" s="102"/>
       <c r="K24" s="102"/>
       <c r="L24" s="102"/>
@@ -6081,9 +6081,9 @@
       <c r="W25" s="102"/>
     </row>
     <row r="26" spans="7:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="G26" s="158"/>
-      <c r="H26" s="151"/>
-      <c r="I26" s="151"/>
+      <c r="G26" s="169"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
       <c r="J26" s="102"/>
       <c r="K26" s="102"/>
       <c r="L26" s="102"/>
@@ -6128,14 +6128,14 @@
       <c r="M28" s="102"/>
       <c r="N28" s="102"/>
       <c r="O28" s="102"/>
-      <c r="P28" s="158"/>
-      <c r="Q28" s="151"/>
-      <c r="R28" s="151"/>
+      <c r="P28" s="169"/>
+      <c r="Q28" s="158"/>
+      <c r="R28" s="158"/>
       <c r="S28" s="102"/>
-      <c r="T28" s="158"/>
-      <c r="U28" s="151"/>
-      <c r="V28" s="151"/>
-      <c r="W28" s="151"/>
+      <c r="T28" s="169"/>
+      <c r="U28" s="158"/>
+      <c r="V28" s="158"/>
+      <c r="W28" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -6177,14 +6177,14 @@
   <sheetData>
     <row r="1" spans="2:8" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="100"/>
-      <c r="C1" s="156" t="s">
+      <c r="C1" s="163" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="102"/>
@@ -6307,12 +6307,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="161" t="s">
+      <c r="C1" s="172" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
     </row>
     <row r="2" spans="2:11" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
@@ -6335,10 +6335,10 @@
       <c r="E6" s="103"/>
     </row>
     <row r="7" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="173" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="151"/>
+      <c r="C7" s="158"/>
       <c r="G7" s="103" t="s">
         <v>103</v>
       </c>
@@ -6447,13 +6447,13 @@
     <row r="1" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="105"/>
       <c r="C1" s="106"/>
-      <c r="D1" s="161" t="s">
+      <c r="D1" s="172" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="105"/>
@@ -6617,12 +6617,12 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="151"/>
-      <c r="M3" s="151"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="158"/>
+      <c r="M3" s="158"/>
     </row>
     <row r="4" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="92"/>

</xml_diff>